<commit_message>
committing changes to experiment controller, adding buttons to control next trial, printing out the start chambers and choice chambers, and right/left choices
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/experiment_controller/Randomized _Trials_Training.xlsx
+++ b/src/omniroute_operation/src/experiment_controller/Randomized _Trials_Training.xlsx
@@ -62,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -104,12 +104,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,7 +148,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -172,10 +166,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -199,10 +189,13 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H37" activeCellId="0" sqref="H37"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -217,7 +210,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -234,9 +227,9 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.530383502080494</v>
+      <c r="E2" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.82658701946604</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -252,9 +245,9 @@
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.342794373994108</v>
+      <c r="E3" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.0798788227293913</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,9 +263,9 @@
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.904466131146331</v>
+      <c r="E4" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.748038191960711</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -288,9 +281,9 @@
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.517453572290894</v>
+      <c r="E5" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.282603320836111</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -306,9 +299,9 @@
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.790555866088295</v>
+      <c r="E6" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.0619064683861887</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -324,9 +317,9 @@
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.0164614385372193</v>
+      <c r="E7" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.324858855546115</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -342,9 +335,9 @@
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.951924657700507</v>
+      <c r="E8" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.981874821516418</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -360,9 +353,9 @@
       <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.358111373653736</v>
+      <c r="E9" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.127807411027764</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -378,9 +371,9 @@
       <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.940555082180213</v>
+      <c r="E10" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.520953757935752</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -396,9 +389,9 @@
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.775692142300945</v>
+      <c r="E11" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.839356373708258</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -414,9 +407,9 @@
       <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.646646940419021</v>
+      <c r="E12" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.0769444133270275</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -432,9 +425,9 @@
       <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.487298424191798</v>
+      <c r="E13" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.56513922783357</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -450,9 +443,9 @@
       <c r="D14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.0373888251067349</v>
+      <c r="E14" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.471701395094663</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,9 +461,9 @@
       <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.301291028166087</v>
+      <c r="E15" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.102230250146701</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -486,9 +479,9 @@
       <c r="D16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.891667650482449</v>
+      <c r="E16" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.291737402209627</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -504,9 +497,9 @@
       <c r="D17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.74643199018764</v>
+      <c r="E17" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.288567060330197</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -522,9 +515,9 @@
       <c r="D18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.388292914195976</v>
+      <c r="E18" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.25954383760975</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -540,9 +533,9 @@
       <c r="D19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.933520139486036</v>
+      <c r="E19" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.0238815552837897</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -558,9 +551,9 @@
       <c r="D20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.441550640295902</v>
+      <c r="E20" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.607914743708082</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -576,9 +569,9 @@
       <c r="D21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.855322771937168</v>
+      <c r="E21" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.14435831514814</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -594,9 +587,9 @@
       <c r="D22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.374443785463942</v>
+      <c r="E22" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.879322410542592</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,9 +605,9 @@
       <c r="D23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.693393400240411</v>
+      <c r="E23" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.160695129431829</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -630,9 +623,9 @@
       <c r="D24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.329132856182431</v>
+      <c r="E24" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.582411657942993</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -648,9 +641,9 @@
       <c r="D25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.232324511020216</v>
+      <c r="E25" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.437316542184763</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -666,9 +659,9 @@
       <c r="D26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.829043045857863</v>
+      <c r="E26" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.742730804255564</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -684,9 +677,9 @@
       <c r="D27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.288166874679335</v>
+      <c r="E27" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.0205801515546295</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -702,9 +695,9 @@
       <c r="D28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.0526412977624601</v>
+      <c r="E28" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.393637698389443</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -720,9 +713,9 @@
       <c r="D29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.401470194613358</v>
+      <c r="E29" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.277554577629597</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -738,9 +731,9 @@
       <c r="D30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.491301356713941</v>
+      <c r="E30" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.461550493526699</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -756,9 +749,9 @@
       <c r="D31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.286488761778691</v>
+      <c r="E31" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.020952844280283</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -774,9 +767,9 @@
       <c r="D32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.243147263386411</v>
+      <c r="E32" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.132008275226149</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,9 +785,9 @@
       <c r="D33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.123676821979153</v>
+      <c r="E33" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.929152634466833</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,9 +803,9 @@
       <c r="D34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.587728023949482</v>
+      <c r="E34" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.811971468796503</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -828,9 +821,9 @@
       <c r="D35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.257144307407928</v>
+      <c r="E35" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.0178132822864843</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -846,9 +839,9 @@
       <c r="D36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.99188957490445</v>
+      <c r="E36" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.685468565605761</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -858,15 +851,15 @@
       <c r="B37" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.847967022781022</v>
+      <c r="E37" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.840819870251147</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -882,9 +875,9 @@
       <c r="D38" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.807366320152671</v>
+      <c r="E38" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.0308403033036289</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -894,15 +887,15 @@
       <c r="B39" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.2429430087284</v>
+      <c r="E39" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.577348548705039</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -918,9 +911,9 @@
       <c r="D40" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E40" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.940663314993538</v>
+      <c r="E40" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.285590803411794</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,15 +923,15 @@
       <c r="B41" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.103877327392549</v>
+      <c r="E41" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.48422716285611</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -954,9 +947,9 @@
       <c r="D42" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.248437172711686</v>
+      <c r="E42" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.685803057957632</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -972,9 +965,9 @@
       <c r="D43" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E43" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.638332050025332</v>
+      <c r="E43" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.190482749841232</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -990,9 +983,9 @@
       <c r="D44" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.26227590471825</v>
+      <c r="E44" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.720301946495133</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1008,9 +1001,9 @@
       <c r="D45" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.37566975759366</v>
+      <c r="E45" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.74938995800556</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1026,9 +1019,9 @@
       <c r="D46" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E46" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.644053356941688</v>
+      <c r="E46" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.112684293149967</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1044,9 +1037,9 @@
       <c r="D47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E47" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.413581371295381</v>
+      <c r="E47" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.603059676141075</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1062,9 +1055,9 @@
       <c r="D48" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E48" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.186215356448108</v>
+      <c r="E48" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.853308740309478</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1080,9 +1073,9 @@
       <c r="D49" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E49" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.585427480418568</v>
+      <c r="E49" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.26436129563262</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,9 +1091,9 @@
       <c r="D50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E50" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.0247030410459563</v>
+      <c r="E50" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.343402379874323</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1116,9 +1109,9 @@
       <c r="D51" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E51" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.541495594028516</v>
+      <c r="E51" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.19982197660544</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1134,9 +1127,9 @@
       <c r="D52" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E52" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.413200561483442</v>
+      <c r="E52" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.533658367208673</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,9 +1145,9 @@
       <c r="D53" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E53" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.629400640906849</v>
+      <c r="E53" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.966824931669416</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,9 +1163,9 @@
       <c r="D54" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.587246597137395</v>
+      <c r="E54" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.33412157556005</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1188,9 +1181,9 @@
       <c r="D55" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.78120893082209</v>
+      <c r="E55" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.359969161237127</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,9 +1199,9 @@
       <c r="D56" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E56" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.158690265824969</v>
+      <c r="E56" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.210634369005189</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1224,9 +1217,9 @@
       <c r="D57" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E57" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.430817881540091</v>
+      <c r="E57" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.957549854622473</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1242,9 +1235,9 @@
       <c r="D58" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E58" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.41672290838884</v>
+      <c r="E58" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.850711496294736</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1260,9 +1253,9 @@
       <c r="D59" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E59" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.232289926809565</v>
+      <c r="E59" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.603782666373964</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1278,9 +1271,9 @@
       <c r="D60" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E60" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.354009734855532</v>
+      <c r="E60" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.938831643266532</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1296,9 +1289,9 @@
       <c r="D61" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E61" s="0" t="n">
-        <f aca="true">RAND()</f>
-        <v>0.845457523574777</v>
+      <c r="E61" s="1" t="n">
+        <f aca="true">RAND()</f>
+        <v>0.496563844642642</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
committing the new button to close all the doors
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/experiment_controller/Randomized _Trials_Training.xlsx
+++ b/src/omniroute_operation/src/experiment_controller/Randomized _Trials_Training.xlsx
@@ -62,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -104,6 +104,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -148,7 +154,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -166,6 +172,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -189,10 +199,10 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
   </cols>
@@ -229,7 +239,7 @@
       </c>
       <c r="E2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.82658701946604</v>
+        <v>0.916556600625179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -247,7 +257,7 @@
       </c>
       <c r="E3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0798788227293913</v>
+        <v>0.852741287438992</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -265,7 +275,7 @@
       </c>
       <c r="E4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.748038191960711</v>
+        <v>0.950541475993729</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -283,7 +293,7 @@
       </c>
       <c r="E5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.282603320836111</v>
+        <v>0.139891237060051</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -301,7 +311,7 @@
       </c>
       <c r="E6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0619064683861887</v>
+        <v>0.445321973774134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -319,7 +329,7 @@
       </c>
       <c r="E7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.324858855546115</v>
+        <v>0.63083783573602</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -337,7 +347,7 @@
       </c>
       <c r="E8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.981874821516418</v>
+        <v>0.765766999095687</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -355,7 +365,7 @@
       </c>
       <c r="E9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.127807411027764</v>
+        <v>0.870607773788847</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,7 +383,7 @@
       </c>
       <c r="E10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.520953757935752</v>
+        <v>0.178841621760316</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -391,7 +401,7 @@
       </c>
       <c r="E11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.839356373708258</v>
+        <v>0.353371403216737</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -409,7 +419,7 @@
       </c>
       <c r="E12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0769444133270275</v>
+        <v>0.648474403855025</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -427,7 +437,7 @@
       </c>
       <c r="E13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.56513922783357</v>
+        <v>0.791677384598414</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -445,7 +455,7 @@
       </c>
       <c r="E14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.471701395094663</v>
+        <v>0.675580246740055</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -463,7 +473,7 @@
       </c>
       <c r="E15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.102230250146701</v>
+        <v>0.793517361856642</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -481,7 +491,7 @@
       </c>
       <c r="E16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.291737402209627</v>
+        <v>0.769586865593375</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -499,7 +509,7 @@
       </c>
       <c r="E17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.288567060330197</v>
+        <v>0.839835120259146</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,7 +527,7 @@
       </c>
       <c r="E18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.25954383760975</v>
+        <v>0.360640475881317</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,7 +545,7 @@
       </c>
       <c r="E19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0238815552837897</v>
+        <v>0.0728287995557399</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -545,15 +555,15 @@
       <c r="B20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>9</v>
+      <c r="C20" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.607914743708082</v>
+        <v>0.990261914523107</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -571,7 +581,7 @@
       </c>
       <c r="E21" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.14435831514814</v>
+        <v>0.464404282174601</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -589,7 +599,7 @@
       </c>
       <c r="E22" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.879322410542592</v>
+        <v>0.609865301746243</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,7 +617,7 @@
       </c>
       <c r="E23" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.160695129431829</v>
+        <v>0.574323066085991</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,7 +635,7 @@
       </c>
       <c r="E24" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.582411657942993</v>
+        <v>0.409881481379049</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -643,7 +653,7 @@
       </c>
       <c r="E25" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.437316542184763</v>
+        <v>0.731432086206963</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,7 +671,7 @@
       </c>
       <c r="E26" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.742730804255564</v>
+        <v>0.558909170538165</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -679,7 +689,7 @@
       </c>
       <c r="E27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0205801515546295</v>
+        <v>0.792926736276098</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -697,7 +707,7 @@
       </c>
       <c r="E28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.393637698389443</v>
+        <v>0.253755078279516</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -715,7 +725,7 @@
       </c>
       <c r="E29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.277554577629597</v>
+        <v>0.646421364365262</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -733,7 +743,7 @@
       </c>
       <c r="E30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.461550493526699</v>
+        <v>0.274398745852814</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,7 +761,7 @@
       </c>
       <c r="E31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.020952844280283</v>
+        <v>0.211598993830997</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -769,7 +779,7 @@
       </c>
       <c r="E32" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.132008275226149</v>
+        <v>0.6936147901587</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,7 +797,7 @@
       </c>
       <c r="E33" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.929152634466833</v>
+        <v>0.573353355283712</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -805,7 +815,7 @@
       </c>
       <c r="E34" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.811971468796503</v>
+        <v>0.643861172683076</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,7 +833,7 @@
       </c>
       <c r="E35" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0178132822864843</v>
+        <v>0.412555349245124</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -841,7 +851,7 @@
       </c>
       <c r="E36" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.685468565605761</v>
+        <v>0.485232093916949</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -859,7 +869,7 @@
       </c>
       <c r="E37" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.840819870251147</v>
+        <v>0.911013990942806</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -877,7 +887,7 @@
       </c>
       <c r="E38" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0308403033036289</v>
+        <v>0.972959627608388</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -895,7 +905,7 @@
       </c>
       <c r="E39" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.577348548705039</v>
+        <v>0.251038850725021</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -913,7 +923,7 @@
       </c>
       <c r="E40" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.285590803411794</v>
+        <v>0.258765158707333</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -931,7 +941,7 @@
       </c>
       <c r="E41" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.48422716285611</v>
+        <v>0.206703535889601</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -949,7 +959,7 @@
       </c>
       <c r="E42" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.685803057957632</v>
+        <v>0.348812966300471</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -967,7 +977,7 @@
       </c>
       <c r="E43" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.190482749841232</v>
+        <v>0.758917910451821</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -985,7 +995,7 @@
       </c>
       <c r="E44" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.720301946495133</v>
+        <v>0.23764041586582</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,7 +1013,7 @@
       </c>
       <c r="E45" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.74938995800556</v>
+        <v>0.43268167474267</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,7 +1031,7 @@
       </c>
       <c r="E46" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.112684293149967</v>
+        <v>0.983103913303951</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1039,7 +1049,7 @@
       </c>
       <c r="E47" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.603059676141075</v>
+        <v>0.0477914029257015</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1057,7 +1067,7 @@
       </c>
       <c r="E48" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.853308740309478</v>
+        <v>0.599157629993084</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,7 +1085,7 @@
       </c>
       <c r="E49" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.26436129563262</v>
+        <v>0.238748837268812</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,7 +1103,7 @@
       </c>
       <c r="E50" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.343402379874323</v>
+        <v>0.279480430999217</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1111,7 +1121,7 @@
       </c>
       <c r="E51" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.19982197660544</v>
+        <v>0.144563393733033</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1129,7 +1139,7 @@
       </c>
       <c r="E52" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.533658367208673</v>
+        <v>0.463584490905285</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1139,15 +1149,15 @@
       <c r="B53" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>9</v>
+      <c r="C53" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E53" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.966824931669416</v>
+        <v>0.58278211739393</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1165,7 +1175,7 @@
       </c>
       <c r="E54" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.33412157556005</v>
+        <v>0.424381814355001</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1183,7 +1193,7 @@
       </c>
       <c r="E55" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.359969161237127</v>
+        <v>0.197381054832317</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1201,7 +1211,7 @@
       </c>
       <c r="E56" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.210634369005189</v>
+        <v>0.0425684456308391</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1211,15 +1221,15 @@
       <c r="B57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>9</v>
+      <c r="C57" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E57" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.957549854622473</v>
+        <v>0.921900631168322</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1237,7 +1247,7 @@
       </c>
       <c r="E58" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.850711496294736</v>
+        <v>0.404328871706495</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1255,7 +1265,7 @@
       </c>
       <c r="E59" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.603782666373964</v>
+        <v>0.00214742443497207</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,7 +1283,7 @@
       </c>
       <c r="E60" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.938831643266532</v>
+        <v>0.577154142274502</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1291,7 +1301,7 @@
       </c>
       <c r="E61" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.496563844642642</v>
+        <v>0.714073971139941</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
committing chabges to experiment controller
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/experiment_controller/Randomized _Trials_Training.xlsx
+++ b/src/omniroute_operation/src/experiment_controller/Randomized _Trials_Training.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="11">
   <si>
     <t xml:space="preserve">Left_Cue</t>
   </si>
@@ -62,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -104,6 +104,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -154,7 +160,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -179,6 +185,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -199,10 +209,10 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
+      <selection pane="topLeft" activeCell="G56" activeCellId="0" sqref="G56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
   </cols>
@@ -239,7 +249,7 @@
       </c>
       <c r="E2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.916556600625179</v>
+        <v>0.686141954779627</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -257,7 +267,7 @@
       </c>
       <c r="E3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.852741287438992</v>
+        <v>0.355105692738254</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -275,7 +285,7 @@
       </c>
       <c r="E4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.950541475993729</v>
+        <v>0.776955535326868</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -293,7 +303,7 @@
       </c>
       <c r="E5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.139891237060051</v>
+        <v>0.43851442072113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -311,7 +321,7 @@
       </c>
       <c r="E6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.445321973774134</v>
+        <v>0.33146015771705</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -329,7 +339,7 @@
       </c>
       <c r="E7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.63083783573602</v>
+        <v>0.245078704815848</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -347,7 +357,7 @@
       </c>
       <c r="E8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.765766999095687</v>
+        <v>0.859725101121004</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -365,7 +375,7 @@
       </c>
       <c r="E9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.870607773788847</v>
+        <v>0.201016985765358</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -383,7 +393,7 @@
       </c>
       <c r="E10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.178841621760316</v>
+        <v>0.733116813522068</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,7 +411,7 @@
       </c>
       <c r="E11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.353371403216737</v>
+        <v>0.452734203108763</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -419,7 +429,7 @@
       </c>
       <c r="E12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.648474403855025</v>
+        <v>0.118761264329599</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -437,7 +447,7 @@
       </c>
       <c r="E13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.791677384598414</v>
+        <v>0.795589090707443</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,7 +465,7 @@
       </c>
       <c r="E14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.675580246740055</v>
+        <v>0.482363792233098</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -473,7 +483,7 @@
       </c>
       <c r="E15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.793517361856642</v>
+        <v>0.790417886325369</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,15 +501,15 @@
       </c>
       <c r="E16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.769586865593375</v>
+        <v>0.386179297316717</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>6</v>
+      <c r="A17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -509,14 +519,14 @@
       </c>
       <c r="E17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.839835120259146</v>
+        <v>0.536675952706156</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -527,15 +537,15 @@
       </c>
       <c r="E18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.360640475881317</v>
+        <v>0.628886507640826</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>5</v>
+      <c r="A19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>7</v>
@@ -545,17 +555,17 @@
       </c>
       <c r="E19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0728287995557399</v>
+        <v>0.790903066049355</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="A20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -563,7 +573,7 @@
       </c>
       <c r="E20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.990261914523107</v>
+        <v>0.221594772725311</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -581,7 +591,7 @@
       </c>
       <c r="E21" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.464404282174601</v>
+        <v>0.22075340054702</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -599,7 +609,7 @@
       </c>
       <c r="E22" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.609865301746243</v>
+        <v>0.68820050195494</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -617,7 +627,7 @@
       </c>
       <c r="E23" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.574323066085991</v>
+        <v>0.733569362245582</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -635,7 +645,7 @@
       </c>
       <c r="E24" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.409881481379049</v>
+        <v>0.940655191961522</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,7 +663,7 @@
       </c>
       <c r="E25" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.731432086206963</v>
+        <v>0.50297346040839</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,7 +681,7 @@
       </c>
       <c r="E26" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.558909170538165</v>
+        <v>0.157693809002104</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -689,7 +699,7 @@
       </c>
       <c r="E27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.792926736276098</v>
+        <v>0.683065820688122</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,7 +717,7 @@
       </c>
       <c r="E28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.253755078279516</v>
+        <v>0.950916489892947</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,7 +735,7 @@
       </c>
       <c r="E29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.646421364365262</v>
+        <v>0.345738217455119</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -743,7 +753,7 @@
       </c>
       <c r="E30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.274398745852814</v>
+        <v>0.190396964034661</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -761,7 +771,7 @@
       </c>
       <c r="E31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.211598993830997</v>
+        <v>0.78271055666177</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -779,7 +789,7 @@
       </c>
       <c r="E32" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.6936147901587</v>
+        <v>0.677543652204444</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -797,7 +807,7 @@
       </c>
       <c r="E33" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.573353355283712</v>
+        <v>0.840656276655074</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,7 +825,7 @@
       </c>
       <c r="E34" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.643861172683076</v>
+        <v>0.807262830855534</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -833,7 +843,7 @@
       </c>
       <c r="E35" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.412555349245124</v>
+        <v>0.726777196553229</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,7 +861,7 @@
       </c>
       <c r="E36" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.485232093916949</v>
+        <v>0.699348481937344</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,7 +879,7 @@
       </c>
       <c r="E37" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.911013990942806</v>
+        <v>0.793860602813886</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,7 +897,7 @@
       </c>
       <c r="E38" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.972959627608388</v>
+        <v>0.718708016426065</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -905,7 +915,7 @@
       </c>
       <c r="E39" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.251038850725021</v>
+        <v>0.0190473992440835</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -923,7 +933,7 @@
       </c>
       <c r="E40" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.258765158707333</v>
+        <v>0.306970664882516</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -941,7 +951,7 @@
       </c>
       <c r="E41" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.206703535889601</v>
+        <v>0.793477103345427</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -959,7 +969,7 @@
       </c>
       <c r="E42" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.348812966300471</v>
+        <v>0.69166152521715</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -977,7 +987,7 @@
       </c>
       <c r="E43" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.758917910451821</v>
+        <v>0.275127447681307</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,7 +1005,7 @@
       </c>
       <c r="E44" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.23764041586582</v>
+        <v>0.236017531981871</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,7 +1023,7 @@
       </c>
       <c r="E45" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.43268167474267</v>
+        <v>0.441584925747424</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1031,7 +1041,7 @@
       </c>
       <c r="E46" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.983103913303951</v>
+        <v>0.864424589512996</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,7 +1059,7 @@
       </c>
       <c r="E47" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0477914029257015</v>
+        <v>0.350352881661225</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1067,7 +1077,7 @@
       </c>
       <c r="E48" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.599157629993084</v>
+        <v>0.690126361306985</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1085,7 +1095,7 @@
       </c>
       <c r="E49" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.238748837268812</v>
+        <v>0.0951452805470236</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1103,15 +1113,15 @@
       </c>
       <c r="E50" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.279480430999217</v>
+        <v>0.623115368933685</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>6</v>
+      <c r="A51" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>7</v>
@@ -1121,7 +1131,7 @@
       </c>
       <c r="E51" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.144563393733033</v>
+        <v>0.289620573335632</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1139,7 +1149,7 @@
       </c>
       <c r="E52" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.463584490905285</v>
+        <v>0.0532462331646482</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1149,7 +1159,7 @@
       <c r="B53" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -1157,7 +1167,7 @@
       </c>
       <c r="E53" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.58278211739393</v>
+        <v>0.826637320109427</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1175,7 +1185,7 @@
       </c>
       <c r="E54" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.424381814355001</v>
+        <v>0.951307652677652</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,15 +1203,15 @@
       </c>
       <c r="E55" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.197381054832317</v>
+        <v>0.520715470223358</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>9</v>
@@ -1211,7 +1221,7 @@
       </c>
       <c r="E56" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0425684456308391</v>
+        <v>0.0523683076665255</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1221,7 +1231,7 @@
       <c r="B57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -1229,7 +1239,7 @@
       </c>
       <c r="E57" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.921900631168322</v>
+        <v>0.930853510471497</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1247,7 +1257,7 @@
       </c>
       <c r="E58" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.404328871706495</v>
+        <v>0.179110567991632</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1265,7 +1275,7 @@
       </c>
       <c r="E59" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.00214742443497207</v>
+        <v>0.140379916445924</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1283,7 +1293,7 @@
       </c>
       <c r="E60" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.577154142274502</v>
+        <v>0.446537342661643</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,12 +1311,22 @@
       </c>
       <c r="E61" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.714073971139941</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="2"/>
-      <c r="B62" s="4"/>
+        <v>0.0487726115386891</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>

</xml_diff>

<commit_message>
committing new functions for automatically generating the next trials
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/experiment_controller/Randomized _Trials_Training.xlsx
+++ b/src/omniroute_operation/src/experiment_controller/Randomized _Trials_Training.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="10">
   <si>
     <t xml:space="preserve">Left_Cue</t>
   </si>
@@ -46,13 +46,10 @@
     <t xml:space="preserve">White_Noise</t>
   </si>
   <si>
-    <t xml:space="preserve">forced_choice</t>
+    <t xml:space="preserve">choice</t>
   </si>
   <si>
     <t xml:space="preserve">5KHz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choice</t>
   </si>
 </sst>
 </file>
@@ -62,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -104,18 +101,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -160,7 +145,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -178,14 +163,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -209,10 +186,10 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G56" activeCellId="0" sqref="G56"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
   </cols>
@@ -249,7 +226,7 @@
       </c>
       <c r="E2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.686141954779627</v>
+        <v>0.329596593227175</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -267,7 +244,7 @@
       </c>
       <c r="E3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.355105692738254</v>
+        <v>0.016952922719083</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -285,7 +262,7 @@
       </c>
       <c r="E4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.776955535326868</v>
+        <v>0.600387764932943</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -303,7 +280,7 @@
       </c>
       <c r="E5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.43851442072113</v>
+        <v>0.168915181606931</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -321,7 +298,7 @@
       </c>
       <c r="E6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.33146015771705</v>
+        <v>0.472755850305454</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -339,7 +316,7 @@
       </c>
       <c r="E7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.245078704815848</v>
+        <v>0.951063272987276</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,7 +334,7 @@
       </c>
       <c r="E8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.859725101121004</v>
+        <v>0.623753019058329</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,7 +352,7 @@
       </c>
       <c r="E9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.201016985765358</v>
+        <v>0.102606327679706</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -393,7 +370,7 @@
       </c>
       <c r="E10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.733116813522068</v>
+        <v>0.741797614184631</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -411,7 +388,7 @@
       </c>
       <c r="E11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.452734203108763</v>
+        <v>0.00406675287676786</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,11 +402,11 @@
         <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.118761264329599</v>
+        <v>0.478647924451693</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -443,11 +420,11 @@
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.795589090707443</v>
+        <v>0.866888262125373</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -461,11 +438,11 @@
         <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.482363792233098</v>
+        <v>0.446943695263027</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -479,11 +456,11 @@
         <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.790417886325369</v>
+        <v>0.159250818034401</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,83 +474,83 @@
         <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.386179297316717</v>
+        <v>0.647908544332044</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.536675952706156</v>
+        <v>0.966147405112969</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.628886507640826</v>
+        <v>0.955510339265857</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.790903066049355</v>
+        <v>0.357285290510358</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.221594772725311</v>
+        <v>0.100797549919619</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -587,11 +564,11 @@
         <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E21" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.22075340054702</v>
+        <v>0.517950675067377</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -605,11 +582,11 @@
         <v>9</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E22" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.68820050195494</v>
+        <v>0.397409685164115</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -623,11 +600,11 @@
         <v>9</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E23" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.733569362245582</v>
+        <v>0.932541795483079</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -641,11 +618,11 @@
         <v>9</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E24" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.940655191961522</v>
+        <v>0.679136337377485</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -659,11 +636,11 @@
         <v>9</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E25" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.50297346040839</v>
+        <v>0.352332291839451</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -677,11 +654,11 @@
         <v>7</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E26" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.157693809002104</v>
+        <v>0.733217607343671</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -695,11 +672,11 @@
         <v>7</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.683065820688122</v>
+        <v>0.413449391836979</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,11 +690,11 @@
         <v>7</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.950916489892947</v>
+        <v>0.808851223726924</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -731,11 +708,11 @@
         <v>9</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.345738217455119</v>
+        <v>0.939297256957034</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,11 +726,11 @@
         <v>9</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.190396964034661</v>
+        <v>0.344111365108991</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -767,11 +744,11 @@
         <v>9</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.78271055666177</v>
+        <v>0.413294476010163</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -785,11 +762,11 @@
         <v>9</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E32" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.677543652204444</v>
+        <v>0.252138968407014</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -803,11 +780,11 @@
         <v>7</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E33" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.840656276655074</v>
+        <v>0.939229451030752</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -821,11 +798,11 @@
         <v>7</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E34" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.807262830855534</v>
+        <v>0.694705271196233</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -839,11 +816,11 @@
         <v>9</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E35" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.726777196553229</v>
+        <v>0.365186859829786</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -857,11 +834,11 @@
         <v>7</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E36" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.699348481937344</v>
+        <v>0.433656824437625</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -875,11 +852,11 @@
         <v>9</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E37" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.793860602813886</v>
+        <v>0.877458145826332</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -893,11 +870,11 @@
         <v>7</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E38" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.718708016426065</v>
+        <v>0.459834136476202</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -911,11 +888,11 @@
         <v>9</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E39" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0190473992440835</v>
+        <v>0.672932338978586</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -929,11 +906,11 @@
         <v>7</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.306970664882516</v>
+        <v>0.409916434519815</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,11 +924,11 @@
         <v>9</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E41" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.793477103345427</v>
+        <v>0.578911190594748</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,11 +942,11 @@
         <v>7</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E42" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.69166152521715</v>
+        <v>0.707963927587423</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -983,11 +960,11 @@
         <v>7</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E43" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.275127447681307</v>
+        <v>0.869838820998488</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1001,11 +978,11 @@
         <v>9</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E44" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.236017531981871</v>
+        <v>0.216318793423133</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1019,11 +996,11 @@
         <v>7</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E45" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.441584925747424</v>
+        <v>0.980210333642266</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1037,11 +1014,11 @@
         <v>9</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E46" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.864424589512996</v>
+        <v>0.00731735334725402</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1055,11 +1032,11 @@
         <v>9</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E47" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.350352881661225</v>
+        <v>0.954162849628566</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1073,11 +1050,11 @@
         <v>7</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E48" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.690126361306985</v>
+        <v>0.609677503647595</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,11 +1068,11 @@
         <v>9</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E49" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0951452805470236</v>
+        <v>0.838712169520232</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1109,15 +1086,15 @@
         <v>7</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E50" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.623115368933685</v>
+        <v>0.417904404003124</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B51" s="4" t="s">
@@ -1127,11 +1104,11 @@
         <v>7</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E51" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.289620573335632</v>
+        <v>0.756831296896603</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,11 +1122,11 @@
         <v>9</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E52" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0532462331646482</v>
+        <v>0.714192463381596</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1163,11 +1140,11 @@
         <v>7</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E53" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.826637320109427</v>
+        <v>0.655684143683315</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1181,11 +1158,11 @@
         <v>9</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E54" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.951307652677652</v>
+        <v>0.713991197368178</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1199,11 +1176,11 @@
         <v>7</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E55" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.520715470223358</v>
+        <v>0.998282454998672</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1217,11 +1194,11 @@
         <v>9</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E56" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0523683076665255</v>
+        <v>0.546616059200256</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1235,11 +1212,11 @@
         <v>7</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E57" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.930853510471497</v>
+        <v>0.371796771981873</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,11 +1230,11 @@
         <v>9</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E58" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.179110567991632</v>
+        <v>0.737485331606196</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1271,11 +1248,11 @@
         <v>7</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E59" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.140379916445924</v>
+        <v>0.176191099190853</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1289,11 +1266,11 @@
         <v>9</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E60" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.446537342661643</v>
+        <v>0.850375944480539</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1307,25 +1284,25 @@
         <v>7</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E61" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0487726115386891</v>
+        <v>0.0302317257554264</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" s="6" t="s">
+      <c r="A62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
committing some changes to the training file
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/experiment_controller/Randomized _Trials_Training.xlsx
+++ b/src/omniroute_operation/src/experiment_controller/Randomized _Trials_Training.xlsx
@@ -59,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -101,6 +101,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,7 +157,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -163,6 +175,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -186,12 +206,12 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="G48" activeCellId="0" sqref="G48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -226,7 +246,7 @@
       </c>
       <c r="E2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.329596593227175</v>
+        <v>0.271852539644509</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -244,7 +264,7 @@
       </c>
       <c r="E3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.016952922719083</v>
+        <v>0.467418409007344</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -262,7 +282,7 @@
       </c>
       <c r="E4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.600387764932943</v>
+        <v>0.313978261153749</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -280,7 +300,7 @@
       </c>
       <c r="E5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.168915181606931</v>
+        <v>0.939630941548646</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -298,7 +318,7 @@
       </c>
       <c r="E6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.472755850305454</v>
+        <v>0.20865920880962</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -316,15 +336,15 @@
       </c>
       <c r="E7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.951063272987276</v>
+        <v>0.632291816744031</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
@@ -334,7 +354,7 @@
       </c>
       <c r="E8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.623753019058329</v>
+        <v>0.0450558079224739</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -352,7 +372,7 @@
       </c>
       <c r="E9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.102606327679706</v>
+        <v>0.40302430049773</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -370,7 +390,7 @@
       </c>
       <c r="E10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.741797614184631</v>
+        <v>0.873285277867288</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -380,15 +400,15 @@
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>7</v>
+      <c r="C11" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.00406675287676786</v>
+        <v>0.979407061867371</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -406,7 +426,7 @@
       </c>
       <c r="E12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.478647924451693</v>
+        <v>0.084011924218502</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -424,7 +444,7 @@
       </c>
       <c r="E13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.866888262125373</v>
+        <v>0.286114058399714</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -442,7 +462,7 @@
       </c>
       <c r="E14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.446943695263027</v>
+        <v>0.659638625223202</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,7 +480,7 @@
       </c>
       <c r="E15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.159250818034401</v>
+        <v>0.53986268356579</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -470,15 +490,15 @@
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>9</v>
+      <c r="C16" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.647908544332044</v>
+        <v>0.825835662022366</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,7 +516,7 @@
       </c>
       <c r="E17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.966147405112969</v>
+        <v>0.653611737006254</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -514,7 +534,7 @@
       </c>
       <c r="E18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.955510339265857</v>
+        <v>0.69731062220814</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -532,15 +552,15 @@
       </c>
       <c r="E19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.357285290510358</v>
+        <v>0.899931947997724</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>6</v>
+        <v>6</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>7</v>
@@ -550,7 +570,7 @@
       </c>
       <c r="E20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.100797549919619</v>
+        <v>0.0124852630615665</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +588,7 @@
       </c>
       <c r="E21" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.517950675067377</v>
+        <v>0.498688966623987</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,7 +606,7 @@
       </c>
       <c r="E22" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.397409685164115</v>
+        <v>0.13754017252497</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,7 +624,7 @@
       </c>
       <c r="E23" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.932541795483079</v>
+        <v>0.187240021976191</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,15 +634,15 @@
       <c r="B24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>9</v>
+      <c r="C24" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.679136337377485</v>
+        <v>0.750088625409653</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -640,7 +660,7 @@
       </c>
       <c r="E25" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.352332291839451</v>
+        <v>0.729384504616608</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,7 +678,7 @@
       </c>
       <c r="E26" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.733217607343671</v>
+        <v>0.452018671195818</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,7 +696,7 @@
       </c>
       <c r="E27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.413449391836979</v>
+        <v>0.837396491671744</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -694,7 +714,7 @@
       </c>
       <c r="E28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.808851223726924</v>
+        <v>0.49822032343044</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,7 +732,7 @@
       </c>
       <c r="E29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.939297256957034</v>
+        <v>0.165915034700576</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -722,15 +742,15 @@
       <c r="B30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>9</v>
+      <c r="C30" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.344111365108991</v>
+        <v>0.286069867283756</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -748,7 +768,7 @@
       </c>
       <c r="E31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.413294476010163</v>
+        <v>0.376608505182788</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -766,7 +786,7 @@
       </c>
       <c r="E32" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.252138968407014</v>
+        <v>0.931445323324286</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -784,7 +804,7 @@
       </c>
       <c r="E33" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.939229451030752</v>
+        <v>0.339315912331438</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -802,7 +822,7 @@
       </c>
       <c r="E34" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.694705271196233</v>
+        <v>0.201068821184006</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -820,7 +840,7 @@
       </c>
       <c r="E35" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.365186859829786</v>
+        <v>0.388739758226336</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,7 +858,7 @@
       </c>
       <c r="E36" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.433656824437625</v>
+        <v>0.110927846332295</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -856,7 +876,7 @@
       </c>
       <c r="E37" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.877458145826332</v>
+        <v>0.971248844362761</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -874,7 +894,7 @@
       </c>
       <c r="E38" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.459834136476202</v>
+        <v>0.457447451682631</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -892,7 +912,7 @@
       </c>
       <c r="E39" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.672932338978586</v>
+        <v>0.222524015860513</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,7 +930,7 @@
       </c>
       <c r="E40" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.409916434519815</v>
+        <v>0.871891043630153</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,7 +948,7 @@
       </c>
       <c r="E41" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.578911190594748</v>
+        <v>0.569476277404128</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -946,7 +966,7 @@
       </c>
       <c r="E42" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.707963927587423</v>
+        <v>0.977893361239774</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,7 +984,7 @@
       </c>
       <c r="E43" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.869838820998488</v>
+        <v>0.460791276349094</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -982,15 +1002,15 @@
       </c>
       <c r="E44" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.216318793423133</v>
+        <v>0.456459830887679</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>6</v>
+        <v>6</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>7</v>
@@ -1000,7 +1020,7 @@
       </c>
       <c r="E45" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.980210333642266</v>
+        <v>0.536178432822489</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1018,15 +1038,15 @@
       </c>
       <c r="E46" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.00731735334725402</v>
+        <v>0.302449913787289</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>6</v>
+        <v>6</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
@@ -1036,15 +1056,15 @@
       </c>
       <c r="E47" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.954162849628566</v>
+        <v>0.235412360157136</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>6</v>
+        <v>6</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>7</v>
@@ -1054,7 +1074,7 @@
       </c>
       <c r="E48" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.609677503647595</v>
+        <v>0.570737343174565</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,7 +1092,7 @@
       </c>
       <c r="E49" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.838712169520232</v>
+        <v>0.777612822634249</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,7 +1110,7 @@
       </c>
       <c r="E50" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.417904404003124</v>
+        <v>0.586189875181419</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1108,7 +1128,7 @@
       </c>
       <c r="E51" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.756831296896603</v>
+        <v>0.148245306218242</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1126,7 +1146,7 @@
       </c>
       <c r="E52" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.714192463381596</v>
+        <v>0.374562177171557</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1144,7 +1164,7 @@
       </c>
       <c r="E53" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.655684143683315</v>
+        <v>0.0695139069769995</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1162,7 +1182,7 @@
       </c>
       <c r="E54" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.713991197368178</v>
+        <v>0.58727477245058</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1180,7 +1200,7 @@
       </c>
       <c r="E55" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.998282454998672</v>
+        <v>0.0690211532388085</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1198,7 +1218,7 @@
       </c>
       <c r="E56" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.546616059200256</v>
+        <v>0.308112933091896</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1216,7 +1236,7 @@
       </c>
       <c r="E57" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.371796771981873</v>
+        <v>0.0755393188478728</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1234,7 +1254,7 @@
       </c>
       <c r="E58" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.737485331606196</v>
+        <v>0.758477487775957</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1252,7 +1272,7 @@
       </c>
       <c r="E59" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.176191099190853</v>
+        <v>0.939026143463467</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1270,15 +1290,15 @@
       </c>
       <c r="E60" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.850375944480539</v>
+        <v>0.921074062503251</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>6</v>
+        <v>6</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>7</v>
@@ -1288,7 +1308,7 @@
       </c>
       <c r="E61" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0302317257554264</v>
+        <v>0.733417251851801</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>